<commit_message>
Facebook login by testNG Screenshot
</commit_message>
<xml_diff>
--- a/bin/com/testdata/HalfEbayTestData.xlsx
+++ b/bin/com/testdata/HalfEbayTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation\TestNg\src\com\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3C93CD-3F36-4797-AAF4-37E50E6D8689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982481DE-B2A9-4DB0-9F9B-73B4D16ACE0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" xr2:uid="{14B856D6-A4FE-4DAB-B050-583781E2AF74}"/>
   </bookViews>
@@ -441,7 +441,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>